<commit_message>
Update scores for evolution algorithm
The evolution algorithm was revised, so testing was done to change the excel spreadsheet.
</commit_message>
<xml_diff>
--- a/Scores.xlsx
+++ b/Scores.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -409,7 +408,7 @@
   <dimension ref="A1:AY23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AF26" sqref="AF26"/>
+      <selection activeCell="Z23" sqref="Z23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +635,7 @@
         <v>1</v>
       </c>
       <c r="Z3">
-        <v>200</v>
+        <v>3040</v>
       </c>
       <c r="AA3">
         <v>1</v>
@@ -749,7 +748,7 @@
         <v>2</v>
       </c>
       <c r="Z4">
-        <v>200</v>
+        <v>2350</v>
       </c>
       <c r="AA4">
         <v>1</v>
@@ -862,7 +861,7 @@
         <v>3</v>
       </c>
       <c r="Z5">
-        <v>200</v>
+        <v>6150</v>
       </c>
       <c r="AA5">
         <v>1</v>
@@ -975,7 +974,7 @@
         <v>4</v>
       </c>
       <c r="Z6">
-        <v>200</v>
+        <v>3360</v>
       </c>
       <c r="AA6">
         <v>1</v>
@@ -1088,7 +1087,7 @@
         <v>5</v>
       </c>
       <c r="Z7">
-        <v>980</v>
+        <v>1630</v>
       </c>
       <c r="AA7">
         <v>1</v>
@@ -1201,7 +1200,7 @@
         <v>6</v>
       </c>
       <c r="Z8">
-        <v>190</v>
+        <v>2710</v>
       </c>
       <c r="AA8">
         <v>1</v>
@@ -1314,7 +1313,7 @@
         <v>7</v>
       </c>
       <c r="Z9">
-        <v>200</v>
+        <v>5580</v>
       </c>
       <c r="AA9">
         <v>1</v>
@@ -1427,7 +1426,7 @@
         <v>8</v>
       </c>
       <c r="Z10">
-        <v>200</v>
+        <v>2720</v>
       </c>
       <c r="AA10">
         <v>1</v>
@@ -1540,7 +1539,7 @@
         <v>9</v>
       </c>
       <c r="Z11">
-        <v>200</v>
+        <v>4940</v>
       </c>
       <c r="AA11">
         <v>1</v>
@@ -1653,7 +1652,7 @@
         <v>10</v>
       </c>
       <c r="Z12">
-        <v>3380</v>
+        <v>960</v>
       </c>
       <c r="AA12">
         <v>1</v>
@@ -1766,7 +1765,7 @@
         <v>11</v>
       </c>
       <c r="Z13">
-        <v>200</v>
+        <v>1120</v>
       </c>
       <c r="AA13">
         <v>1</v>
@@ -1879,7 +1878,7 @@
         <v>12</v>
       </c>
       <c r="Z14">
-        <v>200</v>
+        <v>2860</v>
       </c>
       <c r="AA14">
         <v>1</v>
@@ -1992,7 +1991,7 @@
         <v>13</v>
       </c>
       <c r="Z15">
-        <v>200</v>
+        <v>2710</v>
       </c>
       <c r="AA15">
         <v>1</v>
@@ -2105,7 +2104,7 @@
         <v>14</v>
       </c>
       <c r="Z16">
-        <v>200</v>
+        <v>1650</v>
       </c>
       <c r="AA16">
         <v>1</v>
@@ -2218,7 +2217,7 @@
         <v>15</v>
       </c>
       <c r="Z17">
-        <v>200</v>
+        <v>4250</v>
       </c>
       <c r="AA17">
         <v>1</v>
@@ -2331,7 +2330,7 @@
         <v>16</v>
       </c>
       <c r="Z18">
-        <v>200</v>
+        <v>5020</v>
       </c>
       <c r="AA18">
         <v>1</v>
@@ -2444,7 +2443,7 @@
         <v>17</v>
       </c>
       <c r="Z19">
-        <v>200</v>
+        <v>2570</v>
       </c>
       <c r="AA19">
         <v>1</v>
@@ -2557,7 +2556,7 @@
         <v>18</v>
       </c>
       <c r="Z20">
-        <v>200</v>
+        <v>710</v>
       </c>
       <c r="AA20">
         <v>1</v>
@@ -2670,7 +2669,7 @@
         <v>19</v>
       </c>
       <c r="Z21">
-        <v>200</v>
+        <v>2340</v>
       </c>
       <c r="AA21">
         <v>1</v>
@@ -2783,7 +2782,7 @@
         <v>20</v>
       </c>
       <c r="Z22">
-        <v>200</v>
+        <v>1610</v>
       </c>
       <c r="AA22">
         <v>1</v>
@@ -2909,7 +2908,7 @@
       </c>
       <c r="Z23">
         <f>AVERAGE(Z3:Z22)</f>
-        <v>397.5</v>
+        <v>2914</v>
       </c>
       <c r="AA23">
         <f>AVERAGE(AA3:AA22)</f>

</xml_diff>